<commit_message>
Added batch number wise stock and landscape reports
</commit_message>
<xml_diff>
--- a/app/data/excel/items.xlsx
+++ b/app/data/excel/items.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>code</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Amul ICE CREAM</t>
+  </si>
+  <si>
+    <t>brand name</t>
+  </si>
+  <si>
+    <t>manufacture by</t>
+  </si>
+  <si>
+    <t>Amul</t>
   </si>
 </sst>
 </file>
@@ -378,21 +387,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,16 +412,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -417,12 +435,18 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>